<commit_message>
Update PDF metadata and optimize file size for etiquetas_productos.pdf
</commit_message>
<xml_diff>
--- a/data/productos_con_codigos_cuarta_entrega_solo_para_escanear.xlsx
+++ b/data/productos_con_codigos_cuarta_entrega_solo_para_escanear.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE543FEC-7708-C846-9F91-A2B580E59E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD6AB73-FAC5-7542-A6BF-FC428CE0EBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19980" xr2:uid="{666CB378-938B-7B4C-BE8E-DD88368DB09C}"/>
   </bookViews>
@@ -248,13 +248,13 @@
     <t>Jean Ballion Brown Wash</t>
   </si>
   <si>
-    <t>Jean Semiflare Larisa Limón Wash</t>
-  </si>
-  <si>
-    <t>Jean Semiflare Larisa Lila Wash</t>
-  </si>
-  <si>
-    <t>Jean Semiflare Larisa Celeste Wash</t>
+    <t>Jean S.Flare Larisa Limón W.</t>
+  </si>
+  <si>
+    <t>Jean S.Flare Larisa Celeste W.</t>
+  </si>
+  <si>
+    <t>Jean S.Flare Larisa Lila W.</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,7 +936,7 @@
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
@@ -1060,7 +1060,7 @@
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
         <v>48</v>
@@ -1184,7 +1184,7 @@
         <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
         <v>53</v>
@@ -1246,7 +1246,7 @@
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -1308,7 +1308,7 @@
         <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>

</xml_diff>